<commit_message>
update master sheets and column reference files
</commit_message>
<xml_diff>
--- a/master_sheet_reference_v2.xlsx
+++ b/master_sheet_reference_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mfacade-my.sharepoint.com/personal/jeremy_yap_meinhardtgroup_com/Documents/Python/lighthouse_dash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="523" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A4BFB31-FABD-45A4-892D-F4EC6CF25CF5}"/>
+  <xr:revisionPtr revIDLastSave="588" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D08CD60-5CCD-4ECC-ACC9-4C5103948386}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="9" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
+    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11235" firstSheet="6" activeTab="8" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;M Schedule" sheetId="1" r:id="rId1"/>
@@ -21,10 +21,11 @@
     <sheet name="D&amp;C - HSE &amp; Welfare" sheetId="8" r:id="rId6"/>
     <sheet name="Innovation &amp; Technology" sheetId="9" r:id="rId7"/>
     <sheet name="D&amp;C - Construction" sheetId="6" r:id="rId8"/>
-    <sheet name="Design &amp; Technical" sheetId="4" r:id="rId9"/>
-    <sheet name="Strategy &amp; Operations" sheetId="10" r:id="rId10"/>
-    <sheet name="Glossary&amp;Definitions" sheetId="12" r:id="rId11"/>
-    <sheet name="Visuals Menu" sheetId="11" r:id="rId12"/>
+    <sheet name="Strategy &amp; Operations" sheetId="10" r:id="rId9"/>
+    <sheet name="Design &amp; Technical" sheetId="4" r:id="rId10"/>
+    <sheet name="AssessmentSummary" sheetId="13" r:id="rId11"/>
+    <sheet name="Glossary&amp;Definitions" sheetId="12" r:id="rId12"/>
+    <sheet name="Visuals Menu" sheetId="11" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="121">
   <si>
     <t>Visual</t>
   </si>
@@ -382,22 +383,34 @@
     <t>Glossary&amp;Definitions</t>
   </si>
   <si>
-    <t>Position Vacant</t>
-  </si>
-  <si>
-    <t>Position Missing</t>
-  </si>
-  <si>
     <t>Name of the Policy</t>
   </si>
   <si>
-    <t>Criticality (Y/N)</t>
-  </si>
-  <si>
-    <t>Availability (Y/N)</t>
-  </si>
-  <si>
     <t>Name of the Technical Platform</t>
+  </si>
+  <si>
+    <t>Criticality Policies (Y/N)</t>
+  </si>
+  <si>
+    <t>Availability Policies (Y/N)</t>
+  </si>
+  <si>
+    <t>Criticality Technical (Y/N)</t>
+  </si>
+  <si>
+    <t>Availability Technical (Y/N)</t>
+  </si>
+  <si>
+    <t>Remarks</t>
+  </si>
+  <si>
+    <t>AssessmentSummary</t>
+  </si>
+  <si>
+    <t>DevCoAssessmentInput(S&amp;O)</t>
+  </si>
+  <si>
+    <t>Score</t>
   </si>
 </sst>
 </file>
@@ -795,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E651967B-4962-44AC-8FC1-D4F6809FC53E}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -896,6 +909,22 @@
         <v>60</v>
       </c>
       <c r="C9" s="4"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -916,16 +945,17 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D67D97-B087-4CE0-BB50-05A1992E2859}">
-  <dimension ref="A1:D16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34921496-A0A7-47F9-8DE9-DF05A8622000}">
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -941,130 +971,90 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>92</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B9" t="s">
-        <v>111</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B10" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B11" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>99</v>
-      </c>
-      <c r="B12" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B13" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B14" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>99</v>
-      </c>
-      <c r="B15" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>99</v>
-      </c>
-      <c r="B16" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{10561AED-7A60-4961-BD19-7A4144646A11}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FD68BCFF-90EB-4D8E-B0B1-94E87D7AAC20}">
           <x14:formula1>
             <xm:f>'Visuals Menu'!$A$2:$A$38</xm:f>
           </x14:formula1>
@@ -1077,6 +1067,41 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FB07631-8BD3-49F7-8B83-F2FEBE9985BB}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q17" sqref="Q17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9321A425-4E67-4A55-A6FD-A95196A76FE7}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1123,7 +1148,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D39D204-9365-4464-B2E0-CCC34DC31E80}">
   <dimension ref="A1:A38"/>
   <sheetViews>
@@ -1336,10 +1361,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFB6B33-7153-4BEA-BE79-FA61CA62073D}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:B8"/>
+      <selection activeCell="A16" sqref="A16:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1462,6 +1487,30 @@
       </c>
       <c r="B14" t="s">
         <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1483,10 +1532,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3154CFEB-030A-4FB8-A6DD-5CE49306108D}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B14" sqref="B14:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1594,11 +1643,29 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1619,10 +1686,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FEF6E34-0E07-439B-B3C5-72427B39FD07}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="B11" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1717,6 +1784,22 @@
       </c>
       <c r="B10" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1738,10 +1821,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECA5EB9-4C80-4C7C-BD32-47D2E1728966}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B15" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1865,6 +1948,22 @@
       </c>
       <c r="B14" t="s">
         <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B16" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -1886,15 +1985,15 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F64CC8F8-7393-471E-9562-88A0C3211012}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="B19" sqref="B19:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="4.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
@@ -2046,6 +2145,22 @@
       </c>
       <c r="B18" t="s">
         <v>87</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>72</v>
+      </c>
+      <c r="B19" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2068,10 +2183,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98C8979-387A-4059-8F44-156B7E450536}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A9" sqref="A9:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2146,6 +2261,22 @@
       </c>
       <c r="B8" t="s">
         <v>92</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2167,10 +2298,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A535A6DC-85F0-42C2-9B34-850413E49A7C}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="A13" sqref="A13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2276,6 +2407,22 @@
       </c>
       <c r="B12" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2296,17 +2443,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34921496-A0A7-47F9-8DE9-DF05A8622000}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D67D97-B087-4CE0-BB50-05A1992E2859}">
+  <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2322,90 +2468,179 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>95</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="B11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>99</v>
+      </c>
+      <c r="B12" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>99</v>
+      </c>
+      <c r="B13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>99</v>
+      </c>
+      <c r="B14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B16" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B21" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>98</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{FD68BCFF-90EB-4D8E-B0B1-94E87D7AAC20}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{10561AED-7A60-4961-BD19-7A4144646A11}">
           <x14:formula1>
             <xm:f>'Visuals Menu'!$A$2:$A$38</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
Added org chart columns
</commit_message>
<xml_diff>
--- a/master_sheet_reference_v2.xlsx
+++ b/master_sheet_reference_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mfacade-my.sharepoint.com/personal/jeremy_yap_meinhardtgroup_com/Documents/Python/lighthouse_dash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="588" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D08CD60-5CCD-4ECC-ACC9-4C5103948386}"/>
+  <xr:revisionPtr revIDLastSave="600" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7DC186D-AC7B-40B3-BF6E-FD467EA1274E}"/>
   <bookViews>
-    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11235" firstSheet="6" activeTab="8" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="8" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;M Schedule" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="126">
   <si>
     <t>Visual</t>
   </si>
@@ -411,6 +411,21 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>EmployeeID</t>
+  </si>
+  <si>
+    <t>ManagerID</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Sub-Label</t>
   </si>
 </sst>
 </file>
@@ -814,16 +829,16 @@
       <selection activeCell="B10" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -834,7 +849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>42</v>
       </c>
@@ -845,7 +860,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
@@ -856,7 +871,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -865,7 +880,7 @@
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>44</v>
       </c>
@@ -874,7 +889,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>42</v>
       </c>
@@ -883,7 +898,7 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>42</v>
       </c>
@@ -892,7 +907,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
@@ -901,7 +916,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>42</v>
       </c>
@@ -910,7 +925,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>44</v>
       </c>
@@ -918,7 +933,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
@@ -952,14 +967,14 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -969,7 +984,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -977,7 +992,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -985,7 +1000,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -993,7 +1008,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -1001,7 +1016,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -1009,7 +1024,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -1017,7 +1032,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>95</v>
       </c>
@@ -1025,7 +1040,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -1033,7 +1048,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>93</v>
       </c>
@@ -1041,7 +1056,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>93</v>
       </c>
@@ -1074,12 +1089,12 @@
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1087,7 +1102,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>118</v>
       </c>
@@ -1109,9 +1124,9 @@
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1119,7 +1134,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -1127,7 +1142,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -1135,7 +1150,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>110</v>
       </c>
@@ -1156,197 +1171,197 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1367,14 +1382,14 @@
       <selection activeCell="A16" sqref="A16:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="28.85546875" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1385,7 +1400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
@@ -1393,7 +1408,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
@@ -1401,7 +1416,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
@@ -1409,7 +1424,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>44</v>
       </c>
@@ -1417,7 +1432,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
@@ -1425,7 +1440,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -1433,7 +1448,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
@@ -1441,7 +1456,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
@@ -1449,7 +1464,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
@@ -1457,7 +1472,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -1465,7 +1480,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -1473,7 +1488,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>42</v>
       </c>
@@ -1481,7 +1496,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -1489,7 +1504,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
@@ -1497,7 +1512,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>44</v>
       </c>
@@ -1505,7 +1520,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
@@ -1538,13 +1553,13 @@
       <selection activeCell="B14" sqref="B14:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="24.33203125" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1555,7 +1570,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>61</v>
       </c>
@@ -1563,7 +1578,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>61</v>
       </c>
@@ -1571,7 +1586,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>63</v>
       </c>
@@ -1579,7 +1594,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>63</v>
       </c>
@@ -1587,7 +1602,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>63</v>
       </c>
@@ -1595,7 +1610,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1603,7 +1618,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -1611,7 +1626,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -1619,7 +1634,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -1627,7 +1642,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -1635,7 +1650,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -1643,7 +1658,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>63</v>
       </c>
@@ -1651,7 +1666,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -1659,7 +1674,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>63</v>
       </c>
@@ -1692,15 +1707,15 @@
       <selection activeCell="B11" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1714,7 +1729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -1722,7 +1737,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -1730,7 +1745,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -1738,7 +1753,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -1746,7 +1761,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1754,7 +1769,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -1762,7 +1777,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -1770,7 +1785,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -1778,7 +1793,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1786,7 +1801,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1794,7 +1809,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1827,14 +1842,14 @@
       <selection activeCell="B15" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1846,7 +1861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -1854,7 +1869,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -1862,7 +1877,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1870,7 +1885,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -1878,7 +1893,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1886,7 +1901,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -1894,7 +1909,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -1902,7 +1917,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -1910,7 +1925,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1918,7 +1933,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1926,7 +1941,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1934,7 +1949,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -1942,7 +1957,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -1950,7 +1965,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -1958,7 +1973,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -1991,15 +2006,15 @@
       <selection activeCell="B19" sqref="B19:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2011,7 +2026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -2019,7 +2034,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -2027,7 +2042,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -2035,7 +2050,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -2043,7 +2058,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -2051,7 +2066,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -2059,7 +2074,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -2067,7 +2082,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -2075,7 +2090,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -2083,7 +2098,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -2091,7 +2106,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -2099,7 +2114,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -2107,7 +2122,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -2115,7 +2130,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -2123,7 +2138,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -2131,7 +2146,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -2139,7 +2154,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -2147,7 +2162,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -2155,7 +2170,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -2189,14 +2204,14 @@
       <selection activeCell="A9" sqref="A9:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2207,7 +2222,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -2215,7 +2230,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -2223,7 +2238,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -2231,7 +2246,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -2239,7 +2254,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -2247,7 +2262,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -2255,7 +2270,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -2263,7 +2278,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -2271,7 +2286,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -2304,14 +2319,14 @@
       <selection activeCell="A13" sqref="A13:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2321,7 +2336,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -2329,7 +2344,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -2337,7 +2352,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -2345,7 +2360,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -2353,7 +2368,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -2361,7 +2376,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -2369,7 +2384,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -2377,7 +2392,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -2385,7 +2400,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -2393,7 +2408,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -2401,7 +2416,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -2409,7 +2424,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -2417,7 +2432,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -2444,19 +2459,19 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D67D97-B087-4CE0-BB50-05A1992E2859}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="B23" sqref="B23:B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2466,7 +2481,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -2474,7 +2489,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -2482,7 +2497,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -2490,7 +2505,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -2498,7 +2513,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>99</v>
       </c>
@@ -2506,7 +2521,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -2514,7 +2529,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -2522,7 +2537,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -2530,7 +2545,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -2538,7 +2553,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>99</v>
       </c>
@@ -2546,7 +2561,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>99</v>
       </c>
@@ -2554,7 +2569,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -2562,7 +2577,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -2570,7 +2585,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -2578,7 +2593,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>98</v>
       </c>
@@ -2586,7 +2601,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>119</v>
       </c>
@@ -2594,7 +2609,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -2602,7 +2617,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -2610,7 +2625,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -2618,7 +2633,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>98</v>
       </c>
@@ -2626,12 +2641,52 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>98</v>
       </c>
       <c r="B22" t="s">
         <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>99</v>
+      </c>
+      <c r="B24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>99</v>
+      </c>
+      <c r="B25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>99</v>
+      </c>
+      <c r="B26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B27" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -2644,7 +2699,7 @@
           <x14:formula1>
             <xm:f>'Visuals Menu'!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>D1:D1048576</xm:sqref>
+          <xm:sqref>D1:D1048576 B23</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
updated to include schedule matrix data
</commit_message>
<xml_diff>
--- a/master_sheet_reference_v2.xlsx
+++ b/master_sheet_reference_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mfacade-my.sharepoint.com/personal/jeremy_yap_meinhardtgroup_com/Documents/Python/lighthouse_dash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="600" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D7DC186D-AC7B-40B3-BF6E-FD467EA1274E}"/>
+  <xr:revisionPtr revIDLastSave="613" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9902199-636B-4056-BDD8-4A90422ACD3E}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="8" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
+    <workbookView xWindow="-4755" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;M Schedule" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="Glossary&amp;Definitions" sheetId="12" r:id="rId12"/>
     <sheet name="Visuals Menu" sheetId="11" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" iterate="1" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="135">
   <si>
     <t>Visual</t>
   </si>
@@ -426,6 +426,33 @@
   </si>
   <si>
     <t>Sub-Label</t>
+  </si>
+  <si>
+    <t>ProjectID</t>
+  </si>
+  <si>
+    <t>ForecastCompletionYear</t>
+  </si>
+  <si>
+    <t>ProjectType</t>
+  </si>
+  <si>
+    <t>ProjectStage</t>
+  </si>
+  <si>
+    <t>Criticality</t>
+  </si>
+  <si>
+    <t>DelayInSchedule</t>
+  </si>
+  <si>
+    <t>CostOverrun</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>ProjectValue</t>
   </si>
 </sst>
 </file>
@@ -823,22 +850,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E651967B-4962-44AC-8FC1-D4F6809FC53E}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
@@ -849,7 +876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>42</v>
       </c>
@@ -860,7 +887,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
@@ -871,7 +898,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -880,7 +907,7 @@
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>44</v>
       </c>
@@ -889,7 +916,7 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>42</v>
       </c>
@@ -898,7 +925,7 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>42</v>
       </c>
@@ -907,7 +934,7 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
@@ -916,7 +943,7 @@
       </c>
       <c r="C8" s="4"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>42</v>
       </c>
@@ -925,7 +952,7 @@
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>44</v>
       </c>
@@ -933,12 +960,84 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B11" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B14" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B20" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -967,14 +1066,14 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -984,7 +1083,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>93</v>
       </c>
@@ -992,7 +1091,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>93</v>
       </c>
@@ -1000,7 +1099,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -1008,7 +1107,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -1016,7 +1115,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>93</v>
       </c>
@@ -1024,7 +1123,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -1032,7 +1131,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>95</v>
       </c>
@@ -1040,7 +1139,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>95</v>
       </c>
@@ -1048,7 +1147,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>93</v>
       </c>
@@ -1056,7 +1155,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>93</v>
       </c>
@@ -1089,12 +1188,12 @@
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1102,7 +1201,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>118</v>
       </c>
@@ -1124,9 +1223,9 @@
       <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1134,7 +1233,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>110</v>
       </c>
@@ -1142,7 +1241,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>110</v>
       </c>
@@ -1150,7 +1249,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>110</v>
       </c>
@@ -1171,197 +1270,197 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1382,14 +1481,14 @@
       <selection activeCell="A16" sqref="A16:B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.88671875" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1400,7 +1499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>42</v>
       </c>
@@ -1408,7 +1507,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
@@ -1416,7 +1515,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>44</v>
       </c>
@@ -1424,7 +1523,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>44</v>
       </c>
@@ -1432,7 +1531,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>44</v>
       </c>
@@ -1440,7 +1539,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>42</v>
       </c>
@@ -1448,7 +1547,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>42</v>
       </c>
@@ -1456,7 +1555,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>42</v>
       </c>
@@ -1464,7 +1563,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>42</v>
       </c>
@@ -1472,7 +1571,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>42</v>
       </c>
@@ -1480,7 +1579,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
         <v>42</v>
       </c>
@@ -1488,7 +1587,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>42</v>
       </c>
@@ -1496,7 +1595,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
@@ -1504,7 +1603,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>44</v>
       </c>
@@ -1512,7 +1611,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
         <v>44</v>
       </c>
@@ -1520,7 +1619,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>44</v>
       </c>
@@ -1553,13 +1652,13 @@
       <selection activeCell="B14" sqref="B14:B15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="24.28515625" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="24.33203125" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1570,7 +1669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>61</v>
       </c>
@@ -1578,7 +1677,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>61</v>
       </c>
@@ -1586,7 +1685,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>63</v>
       </c>
@@ -1594,7 +1693,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>63</v>
       </c>
@@ -1602,7 +1701,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>63</v>
       </c>
@@ -1610,7 +1709,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>64</v>
       </c>
@@ -1618,7 +1717,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>64</v>
       </c>
@@ -1626,7 +1725,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>64</v>
       </c>
@@ -1634,7 +1733,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -1642,7 +1741,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>64</v>
       </c>
@@ -1650,7 +1749,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>64</v>
       </c>
@@ -1658,7 +1757,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>63</v>
       </c>
@@ -1666,7 +1765,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>63</v>
       </c>
@@ -1674,7 +1773,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>63</v>
       </c>
@@ -1707,15 +1806,15 @@
       <selection activeCell="B11" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1729,7 +1828,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -1737,7 +1836,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -1745,7 +1844,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>68</v>
       </c>
@@ -1753,7 +1852,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>68</v>
       </c>
@@ -1761,7 +1860,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -1769,7 +1868,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -1777,7 +1876,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -1785,7 +1884,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -1793,7 +1892,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1801,7 +1900,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1809,7 +1908,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -1842,14 +1941,14 @@
       <selection activeCell="B15" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1861,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -1869,7 +1968,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -1877,7 +1976,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -1885,7 +1984,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -1893,7 +1992,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -1901,7 +2000,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -1909,7 +2008,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>72</v>
       </c>
@@ -1917,7 +2016,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -1925,7 +2024,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -1933,7 +2032,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -1941,7 +2040,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>68</v>
       </c>
@@ -1949,7 +2048,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -1957,7 +2056,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>68</v>
       </c>
@@ -1965,7 +2064,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>72</v>
       </c>
@@ -1973,7 +2072,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>72</v>
       </c>
@@ -2006,15 +2105,15 @@
       <selection activeCell="B19" sqref="B19:B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2026,7 +2125,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -2034,7 +2133,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -2042,7 +2141,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -2050,7 +2149,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -2058,7 +2157,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>67</v>
       </c>
@@ -2066,7 +2165,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -2074,7 +2173,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -2082,7 +2181,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>67</v>
       </c>
@@ -2090,7 +2189,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>67</v>
       </c>
@@ -2098,7 +2197,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -2106,7 +2205,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>67</v>
       </c>
@@ -2114,7 +2213,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>67</v>
       </c>
@@ -2122,7 +2221,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>67</v>
       </c>
@@ -2130,7 +2229,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>67</v>
       </c>
@@ -2138,7 +2237,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>67</v>
       </c>
@@ -2146,7 +2245,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>67</v>
       </c>
@@ -2154,7 +2253,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>67</v>
       </c>
@@ -2162,7 +2261,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>72</v>
       </c>
@@ -2170,7 +2269,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -2204,14 +2303,14 @@
       <selection activeCell="A9" sqref="A9:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2222,7 +2321,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>82</v>
       </c>
@@ -2230,7 +2329,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -2238,7 +2337,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -2246,7 +2345,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>83</v>
       </c>
@@ -2254,7 +2353,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>83</v>
       </c>
@@ -2262,7 +2361,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -2270,7 +2369,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>83</v>
       </c>
@@ -2278,7 +2377,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>83</v>
       </c>
@@ -2286,7 +2385,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>83</v>
       </c>
@@ -2319,14 +2418,14 @@
       <selection activeCell="A13" sqref="A13:B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2336,7 +2435,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>67</v>
       </c>
@@ -2344,7 +2443,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -2352,7 +2451,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>67</v>
       </c>
@@ -2360,7 +2459,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>67</v>
       </c>
@@ -2368,7 +2467,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>68</v>
       </c>
@@ -2376,7 +2475,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>67</v>
       </c>
@@ -2384,7 +2483,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>67</v>
       </c>
@@ -2392,7 +2491,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>72</v>
       </c>
@@ -2400,7 +2499,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -2408,7 +2507,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>72</v>
       </c>
@@ -2416,7 +2515,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>72</v>
       </c>
@@ -2424,7 +2523,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>72</v>
       </c>
@@ -2432,7 +2531,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -2461,17 +2560,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D67D97-B087-4CE0-BB50-05A1992E2859}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23:B28"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2481,7 +2580,7 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>98</v>
       </c>
@@ -2489,7 +2588,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>98</v>
       </c>
@@ -2497,7 +2596,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>98</v>
       </c>
@@ -2505,7 +2604,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>99</v>
       </c>
@@ -2513,7 +2612,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>99</v>
       </c>
@@ -2521,7 +2620,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>99</v>
       </c>
@@ -2529,7 +2628,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -2537,7 +2636,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>99</v>
       </c>
@@ -2545,7 +2644,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>99</v>
       </c>
@@ -2553,7 +2652,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>99</v>
       </c>
@@ -2561,7 +2660,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>99</v>
       </c>
@@ -2569,7 +2668,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>99</v>
       </c>
@@ -2577,7 +2676,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>99</v>
       </c>
@@ -2585,7 +2684,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>98</v>
       </c>
@@ -2593,7 +2692,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>98</v>
       </c>
@@ -2601,7 +2700,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>119</v>
       </c>
@@ -2609,7 +2708,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>119</v>
       </c>
@@ -2617,7 +2716,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>119</v>
       </c>
@@ -2625,7 +2724,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>98</v>
       </c>
@@ -2633,7 +2732,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>98</v>
       </c>
@@ -2641,7 +2740,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>98</v>
       </c>
@@ -2649,7 +2748,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>99</v>
       </c>
@@ -2657,7 +2756,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>99</v>
       </c>
@@ -2665,7 +2764,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>99</v>
       </c>
@@ -2673,7 +2772,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>99</v>
       </c>
@@ -2681,7 +2780,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>99</v>
       </c>

</xml_diff>

<commit_message>
catch all for columns from AddDataPoint(P&M)
</commit_message>
<xml_diff>
--- a/master_sheet_reference_v2.xlsx
+++ b/master_sheet_reference_v2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mfacade-my.sharepoint.com/personal/jeremy_yap_meinhardtgroup_com/Documents/Python/lighthouse_dash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="613" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F9902199-636B-4056-BDD8-4A90422ACD3E}"/>
+  <xr:revisionPtr revIDLastSave="619" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8467CA2E-2925-44B8-9A46-A8FEDB624ED5}"/>
   <bookViews>
-    <workbookView xWindow="-4755" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;M Schedule" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
     <sheet name="Glossary&amp;Definitions" sheetId="12" r:id="rId12"/>
     <sheet name="Visuals Menu" sheetId="11" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="191029" iterate="1" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="135">
   <si>
     <t>Visual</t>
   </si>
@@ -850,109 +850,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E651967B-4962-44AC-8FC1-D4F6809FC53E}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>44</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="4"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>44</v>
       </c>
@@ -960,7 +945,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>44</v>
       </c>
@@ -968,7 +953,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>42</v>
       </c>
@@ -976,7 +961,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>42</v>
       </c>
@@ -984,7 +969,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>42</v>
       </c>
@@ -992,7 +977,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>42</v>
       </c>
@@ -1000,7 +985,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>42</v>
       </c>
@@ -1050,7 +1035,7 @@
           <x14:formula1>
             <xm:f>'Visuals Menu'!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C3 B5</xm:sqref>
+          <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
latest code for Intermediate File compiler
</commit_message>
<xml_diff>
--- a/master_sheet_reference_v2.xlsx
+++ b/master_sheet_reference_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mfacade-my.sharepoint.com/personal/jeremy_yap_meinhardtgroup_com/Documents/Python/lighthouse_dash/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chavi.mangla\Dash\lighthouse_dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="619" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8467CA2E-2925-44B8-9A46-A8FEDB624ED5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3C92A8-48D9-4F36-869B-C1C7C58CCDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;M Schedule" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="145">
   <si>
     <t>Visual</t>
   </si>
@@ -453,6 +453,36 @@
   </si>
   <si>
     <t>ProjectValue</t>
+  </si>
+  <si>
+    <t>DevCoAssessmentInput(P&amp;M)</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Total Positions</t>
+  </si>
+  <si>
+    <t>No of Positions Unfullfiled</t>
+  </si>
+  <si>
+    <t>% of Position Unfullfiled</t>
+  </si>
+  <si>
+    <t>Position Vacant</t>
+  </si>
+  <si>
+    <t>Position Missing</t>
+  </si>
+  <si>
+    <t>Name of the Department</t>
+  </si>
+  <si>
+    <t>No of Position Missing</t>
+  </si>
+  <si>
+    <t>DevCoAssessmentInput(I&amp;T)</t>
   </si>
 </sst>
 </file>
@@ -850,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E651967B-4962-44AC-8FC1-D4F6809FC53E}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -885,8 +915,8 @@
       <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>39</v>
+      <c r="B3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1023,6 +1053,22 @@
       </c>
       <c r="B20" t="s">
         <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1035,7 +1081,7 @@
           <x14:formula1>
             <xm:f>'Visuals Menu'!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>B5</xm:sqref>
+          <xm:sqref>B5 B22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1048,7 +1094,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1460,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFB6B33-7153-4BEA-BE79-FA61CA62073D}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:B17"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1493,11 +1539,11 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1610,6 +1656,22 @@
       </c>
       <c r="B17" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1621,7 +1683,7 @@
           <x14:formula1>
             <xm:f>'Visuals Menu'!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C8 C10:C1048576 B10</xm:sqref>
+          <xm:sqref>C1:C8 C10:C1048576 B10 B19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1634,7 +1696,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1707,7 +1769,7 @@
         <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1775,7 +1837,7 @@
           <x14:formula1>
             <xm:f>'Visuals Menu'!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>C1 B3 C3:C6 B8:C8 B10 C10:C1048576</xm:sqref>
+          <xm:sqref>C1 B3 C3:C6 C10:C1048576 B10 C8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1785,10 +1847,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FEF6E34-0E07-439B-B3C5-72427B39FD07}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B12"/>
+      <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1866,7 +1928,7 @@
         <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1899,6 +1961,14 @@
       </c>
       <c r="B12" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1920,10 +1990,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECA5EB9-4C80-4C7C-BD32-47D2E1728966}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B16"/>
+      <selection activeCell="A17" sqref="A17:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2063,6 +2133,14 @@
       </c>
       <c r="B16" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2087,7 +2165,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:B20"/>
+      <selection activeCell="B21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2123,7 +2201,7 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2282,15 +2360,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98C8979-387A-4059-8F44-156B7E450536}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2319,12 +2397,12 @@
         <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
         <v>45</v>
@@ -2332,18 +2410,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2351,7 +2429,7 @@
         <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2359,7 +2437,7 @@
         <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -2367,7 +2445,7 @@
         <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -2375,6 +2453,30 @@
         <v>83</v>
       </c>
       <c r="B10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2400,7 +2502,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:B14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2473,7 +2575,7 @@
         <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2543,15 +2645,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D67D97-B087-4CE0-BB50-05A1992E2859}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="A20" sqref="A20:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2618,7 +2721,7 @@
         <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2771,6 +2874,70 @@
       </c>
       <c r="B27" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "latest code for Intermediate File compiler"
This reverts commit 7e14054e04dc79aab6326397d535a487a6eadc39.
</commit_message>
<xml_diff>
--- a/master_sheet_reference_v2.xlsx
+++ b/master_sheet_reference_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chavi.mangla\Dash\lighthouse_dash\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mfacade-my.sharepoint.com/personal/jeremy_yap_meinhardtgroup_com/Documents/Python/lighthouse_dash/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3C92A8-48D9-4F36-869B-C1C7C58CCDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="619" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8467CA2E-2925-44B8-9A46-A8FEDB624ED5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;M Schedule" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="135">
   <si>
     <t>Visual</t>
   </si>
@@ -453,36 +453,6 @@
   </si>
   <si>
     <t>ProjectValue</t>
-  </si>
-  <si>
-    <t>DevCoAssessmentInput(P&amp;M)</t>
-  </si>
-  <si>
-    <t>Department</t>
-  </si>
-  <si>
-    <t>Total Positions</t>
-  </si>
-  <si>
-    <t>No of Positions Unfullfiled</t>
-  </si>
-  <si>
-    <t>% of Position Unfullfiled</t>
-  </si>
-  <si>
-    <t>Position Vacant</t>
-  </si>
-  <si>
-    <t>Position Missing</t>
-  </si>
-  <si>
-    <t>Name of the Department</t>
-  </si>
-  <si>
-    <t>No of Position Missing</t>
-  </si>
-  <si>
-    <t>DevCoAssessmentInput(I&amp;T)</t>
   </si>
 </sst>
 </file>
@@ -880,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E651967B-4962-44AC-8FC1-D4F6809FC53E}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -915,8 +885,8 @@
       <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B3" t="s">
-        <v>62</v>
+      <c r="B3" s="4" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1053,22 +1023,6 @@
       </c>
       <c r="B20" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B21" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B22" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1081,7 +1035,7 @@
           <x14:formula1>
             <xm:f>'Visuals Menu'!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>B5 B22</xm:sqref>
+          <xm:sqref>B5</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1094,7 +1048,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1506,10 +1460,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFB6B33-7153-4BEA-BE79-FA61CA62073D}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="A16" sqref="A16:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1539,11 +1493,11 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1656,22 +1610,6 @@
       </c>
       <c r="B17" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B18" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="B19" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1683,7 +1621,7 @@
           <x14:formula1>
             <xm:f>'Visuals Menu'!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C8 C10:C1048576 B10 B19</xm:sqref>
+          <xm:sqref>C1:C8 C10:C1048576 B10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1696,7 +1634,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B14" sqref="B14:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1769,7 +1707,7 @@
         <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1837,7 +1775,7 @@
           <x14:formula1>
             <xm:f>'Visuals Menu'!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>C1 B3 C3:C6 C10:C1048576 B10 C8</xm:sqref>
+          <xm:sqref>C1 B3 C3:C6 B8:C8 B10 C10:C1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1847,10 +1785,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FEF6E34-0E07-439B-B3C5-72427B39FD07}">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:B13"/>
+      <selection activeCell="B11" sqref="B11:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1928,7 +1866,7 @@
         <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1961,14 +1899,6 @@
       </c>
       <c r="B12" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B13" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1990,10 +1920,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECA5EB9-4C80-4C7C-BD32-47D2E1728966}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:B17"/>
+      <selection activeCell="B15" sqref="B15:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2133,14 +2063,6 @@
       </c>
       <c r="B16" t="s">
         <v>103</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" t="s">
-        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2165,7 +2087,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="A21:B21"/>
+      <selection activeCell="B19" sqref="B19:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2201,7 +2123,7 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2360,15 +2282,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98C8979-387A-4059-8F44-156B7E450536}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2397,12 +2319,12 @@
         <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
       <c r="B4" t="s">
         <v>45</v>
@@ -2410,18 +2332,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>144</v>
+        <v>83</v>
       </c>
       <c r="B6" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2429,7 +2351,7 @@
         <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2437,7 +2359,7 @@
         <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -2445,7 +2367,7 @@
         <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -2453,30 +2375,6 @@
         <v>83</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>83</v>
-      </c>
-      <c r="B11" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>83</v>
-      </c>
-      <c r="B12" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>83</v>
-      </c>
-      <c r="B13" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2502,7 +2400,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A13" sqref="A13:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2575,7 +2473,7 @@
         <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2645,16 +2543,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D67D97-B087-4CE0-BB50-05A1992E2859}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:B20"/>
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5546875" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2721,7 +2618,7 @@
         <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>62</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2874,70 +2771,6 @@
       </c>
       <c r="B27" t="s">
         <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>99</v>
-      </c>
-      <c r="B28" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>99</v>
-      </c>
-      <c r="B29" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>99</v>
-      </c>
-      <c r="B30" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>99</v>
-      </c>
-      <c r="B31" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>99</v>
-      </c>
-      <c r="B32" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>99</v>
-      </c>
-      <c r="B33" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>99</v>
-      </c>
-      <c r="B34" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>99</v>
-      </c>
-      <c r="B35" t="s">
-        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reapply "latest code for Intermediate File compiler"
This reverts commit eb07a9dfcae12c501add20e62ec22738d88664fc.
</commit_message>
<xml_diff>
--- a/master_sheet_reference_v2.xlsx
+++ b/master_sheet_reference_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mfacade-my.sharepoint.com/personal/jeremy_yap_meinhardtgroup_com/Documents/Python/lighthouse_dash/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chavi.mangla\Dash\lighthouse_dash\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="619" documentId="8_{8B52F1BC-D773-4C97-B9A6-47342E7012CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8467CA2E-2925-44B8-9A46-A8FEDB624ED5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E3C92A8-48D9-4F36-869B-C1C7C58CCDFD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="4" activeTab="6" xr2:uid="{02DDB304-69C4-4CA3-8C49-D9488FBD6A5E}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;M Schedule" sheetId="1" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="145">
   <si>
     <t>Visual</t>
   </si>
@@ -453,6 +453,36 @@
   </si>
   <si>
     <t>ProjectValue</t>
+  </si>
+  <si>
+    <t>DevCoAssessmentInput(P&amp;M)</t>
+  </si>
+  <si>
+    <t>Department</t>
+  </si>
+  <si>
+    <t>Total Positions</t>
+  </si>
+  <si>
+    <t>No of Positions Unfullfiled</t>
+  </si>
+  <si>
+    <t>% of Position Unfullfiled</t>
+  </si>
+  <si>
+    <t>Position Vacant</t>
+  </si>
+  <si>
+    <t>Position Missing</t>
+  </si>
+  <si>
+    <t>Name of the Department</t>
+  </si>
+  <si>
+    <t>No of Position Missing</t>
+  </si>
+  <si>
+    <t>DevCoAssessmentInput(I&amp;T)</t>
   </si>
 </sst>
 </file>
@@ -850,10 +880,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E651967B-4962-44AC-8FC1-D4F6809FC53E}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -885,8 +915,8 @@
       <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>39</v>
+      <c r="B3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1023,6 +1053,22 @@
       </c>
       <c r="B20" t="s">
         <v>134</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B21" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1035,7 +1081,7 @@
           <x14:formula1>
             <xm:f>'Visuals Menu'!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>B5</xm:sqref>
+          <xm:sqref>B5 B22</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1048,7 +1094,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1460,10 +1506,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DFB6B33-7153-4BEA-BE79-FA61CA62073D}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:B17"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1493,11 +1539,11 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1610,6 +1656,22 @@
       </c>
       <c r="B17" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="B19" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1621,7 +1683,7 @@
           <x14:formula1>
             <xm:f>'Visuals Menu'!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>C1:C8 C10:C1048576 B10</xm:sqref>
+          <xm:sqref>C1:C8 C10:C1048576 B10 B19</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1634,7 +1696,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:B15"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1707,7 +1769,7 @@
         <v>64</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1775,7 +1837,7 @@
           <x14:formula1>
             <xm:f>'Visuals Menu'!$A$2:$A$38</xm:f>
           </x14:formula1>
-          <xm:sqref>C1 B3 C3:C6 B8:C8 B10 C10:C1048576</xm:sqref>
+          <xm:sqref>C1 B3 C3:C6 C10:C1048576 B10 C8</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1785,10 +1847,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FEF6E34-0E07-439B-B3C5-72427B39FD07}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B12"/>
+      <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1866,7 +1928,7 @@
         <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -1899,6 +1961,14 @@
       </c>
       <c r="B12" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>67</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -1920,10 +1990,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECA5EB9-4C80-4C7C-BD32-47D2E1728966}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15:B16"/>
+      <selection activeCell="A17" sqref="A17:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2063,6 +2133,14 @@
       </c>
       <c r="B16" t="s">
         <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>67</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2087,7 +2165,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19:B20"/>
+      <selection activeCell="B21" sqref="A21:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2123,7 +2201,7 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -2282,15 +2360,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C98C8979-387A-4059-8F44-156B7E450536}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.44140625" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2319,12 +2397,12 @@
         <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="B4" t="s">
         <v>45</v>
@@ -2332,18 +2410,18 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>144</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2351,7 +2429,7 @@
         <v>83</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2359,7 +2437,7 @@
         <v>83</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -2367,7 +2445,7 @@
         <v>83</v>
       </c>
       <c r="B9" t="s">
-        <v>102</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -2375,6 +2453,30 @@
         <v>83</v>
       </c>
       <c r="B10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B11" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>83</v>
+      </c>
+      <c r="B12" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2400,7 +2502,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:B14"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2473,7 +2575,7 @@
         <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2543,15 +2645,16 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45D67D97-B087-4CE0-BB50-05A1992E2859}">
-  <dimension ref="A1:D27"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="A20" sqref="A20:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="29.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5546875" customWidth="1"/>
     <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2618,7 +2721,7 @@
         <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
@@ -2771,6 +2874,70 @@
       </c>
       <c r="B27" t="s">
         <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>99</v>
+      </c>
+      <c r="B30" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>99</v>
+      </c>
+      <c r="B31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>99</v>
+      </c>
+      <c r="B33" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>99</v>
+      </c>
+      <c r="B34" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>99</v>
+      </c>
+      <c r="B35" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>